<commit_message>
added dqCore.R, icdRD_no and pt_no
</commit_message>
<xml_diff>
--- a/examples/Data/Export/Datenqualitätsreport_ CORD_TestData .xlsx
+++ b/examples/Data/Export/Datenqualitätsreport_ CORD_TestData .xlsx
@@ -352,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -383,182 +383,302 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>P_19285751</t>
+          <t>P_1057020</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>E84.0</t>
+          <t>E70.0</t>
         </is>
       </c>
       <c r="C2">
-        <v>587</v>
+        <v>79254</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Relation  E84.0 - 587  ist im BfArM nicht vorhanden </t>
+          <t xml:space="preserve">Relation  E70.0 - 79254  ist im BfArM nicht vorhanden </t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>P_19285752</t>
+          <t>P_1057020</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>E84.8</t>
+          <t>E70.0</t>
         </is>
       </c>
       <c r="C3">
-        <v>586</v>
+        <v>79254</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Relation  E84.8 - 586  ist im BfArM nicht vorhanden</t>
+          <t xml:space="preserve">Relation  E70.0 - 79254  ist im BfArM nicht vorhanden </t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>P_19285753</t>
+          <t>P_1695115</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>E84.8</t>
+          <t>E70.0</t>
         </is>
       </c>
       <c r="C4">
-        <v>587</v>
+        <v>79254</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve">ICD10 Kodierung  E84.8  ist im BfArm-Mapping nicht enthalten </t>
+          <t xml:space="preserve">Relation  E70.0 - 79254  ist im BfArM nicht vorhanden </t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>P_19285754</t>
+          <t>P_1695115</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>E85.0</t>
+          <t>E70.0</t>
         </is>
       </c>
       <c r="C5">
-        <v>586</v>
+        <v>79254</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Relation  E85.0 - 586  ist im BfArM nicht vorhanden </t>
+          <t xml:space="preserve">Relation  E70.0 - 79254  ist im BfArM nicht vorhanden </t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>P_19285755</t>
+          <t>P_1897170</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>E75.2</t>
+          <t>E70.0</t>
         </is>
       </c>
       <c r="C6">
-        <v>325</v>
+        <v>79254</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Relation  E75.2 - 325  ist im BfArM nicht vorhanden </t>
+          <t xml:space="preserve">Relation  E70.0 - 79254  ist im BfArM nicht vorhanden </t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>P_19285756</t>
+          <t>P_1897170</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>E75.2</t>
+          <t>E70.0</t>
         </is>
       </c>
       <c r="C7">
-        <v>320</v>
+        <v>79254</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Relation  E75.2 - 320  ist im BfArM nicht vorhanden </t>
+          <t xml:space="preserve">Relation  E70.0 - 79254  ist im BfArM nicht vorhanden </t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>P_19285757</t>
+          <t>P_19285751</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>E84.0</t>
         </is>
       </c>
       <c r="C8">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fehlendes ICD10 Code  </t>
+          <t xml:space="preserve">Relation  E84.0 - 587  ist im BfArM nicht vorhanden </t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>P_19285758</t>
+          <t>P_19285752</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>E84.8</t>
         </is>
       </c>
       <c r="C9">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Orpha Kodierung  587  ist im BfArM-Mapping nicht enthalten Fehlendes ICD10 Code  </t>
+          <t>Relation  E84.8 - 586  ist im BfArM nicht vorhanden</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>P_19285759</t>
+          <t>P_19285753</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>E75.2</t>
-        </is>
+          <t>E84.8</t>
+        </is>
+      </c>
+      <c r="C10">
+        <v>587</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t xml:space="preserve">ICD10-Kodierung nicht eindeutig E75.2 </t>
+          <t xml:space="preserve">ICD10 Kodierung  E84.8  ist im BfArm-Mapping nicht enthalten </t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>P_19285754</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>E85.0</t>
+        </is>
+      </c>
+      <c r="C11">
+        <v>586</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Relation  E85.0 - 586  ist im BfArM nicht vorhanden </t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>P_19285755</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>E75.2</t>
+        </is>
+      </c>
+      <c r="C12">
+        <v>325</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Relation  E75.2 - 325  ist im BfArM nicht vorhanden </t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>P_19285756</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>E75.2</t>
+        </is>
+      </c>
+      <c r="C13">
+        <v>320</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Relation  E75.2 - 320  ist im BfArM nicht vorhanden </t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>P_19285757</t>
+        </is>
+      </c>
+      <c r="C14">
+        <v>586</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fehlendes ICD10 Code  </t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>P_19285758</t>
+        </is>
+      </c>
+      <c r="C15">
+        <v>587</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Orpha Kodierung  587  ist im BfArM-Mapping nicht enthalten Fehlendes ICD10 Code  </t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
           <t>P_19285759</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>E75.2</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ICD10-Kodierung nicht eindeutig E75.2 </t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>P_19285759</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
         <is>
           <t>E84.0</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t xml:space="preserve">ICD10-Kodierung nicht eindeutig E84.0 </t>
         </is>
@@ -571,7 +691,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -590,17 +710,27 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>K2_completness_rate</t>
+          <t>completness_rate</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>K2_OrphaCoding_completeness</t>
+          <t>orphaCoding_completeness</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>K3_uniqueness_rate</t>
+          <t>uniqueness_rate</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>icdRd_no</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>pt_no</t>
         </is>
       </c>
     </row>
@@ -620,7 +750,13 @@
         <v>94.44</v>
       </c>
       <c r="E2">
-        <v>98.59999999999999</v>
+        <v>96.59999999999999</v>
+      </c>
+      <c r="F2">
+        <v>36</v>
+      </c>
+      <c r="G2">
+        <v>382</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add Hamburger-Cord List as reference, update code and test data
</commit_message>
<xml_diff>
--- a/examples/Data/Export/Datenqualitätsreport_ CORD_TestData .xlsx
+++ b/examples/Data/Export/Datenqualitätsreport_ CORD_TestData .xlsx
@@ -352,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -383,132 +383,122 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>P_1057020</t>
+          <t>P_19285751</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>E70.0</t>
+          <t>E84.0</t>
         </is>
       </c>
       <c r="C2">
-        <v>79254</v>
+        <v>587</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Relation  E70.0 - 79254  ist im BfArM nicht vorhanden </t>
+          <t xml:space="preserve">Relation  E84.0 - 587  ist im BfArM nicht vorhanden </t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>P_1057020</t>
+          <t>P_19285753</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>E70.0</t>
+          <t>E84.80</t>
         </is>
       </c>
       <c r="C3">
-        <v>79254</v>
+        <v>587</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Relation  E70.0 - 79254  ist im BfArM nicht vorhanden </t>
+          <t xml:space="preserve">Relation  E84.80 - 587  ist im BfArM nicht vorhanden </t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>P_1695115</t>
+          <t>P_19285754</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>E70.0</t>
+          <t>E85.0</t>
         </is>
       </c>
       <c r="C4">
-        <v>79254</v>
+        <v>586</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Relation  E70.0 - 79254  ist im BfArM nicht vorhanden </t>
+          <t xml:space="preserve">Relation  E85.0 - 586  ist im BfArM nicht vorhanden </t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>P_1695115</t>
+          <t>P_19285755</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>E70.0</t>
+          <t>E75.2</t>
         </is>
       </c>
       <c r="C5">
-        <v>79254</v>
+        <v>325</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Relation  E70.0 - 79254  ist im BfArM nicht vorhanden </t>
+          <t xml:space="preserve">Relation  E75.2 - 325  ist im BfArM nicht vorhanden </t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>P_1897170</t>
+          <t>P_19285756</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>E70.0</t>
+          <t>E75.2</t>
         </is>
       </c>
       <c r="C6">
-        <v>79254</v>
+        <v>320</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Relation  E70.0 - 79254  ist im BfArM nicht vorhanden </t>
+          <t xml:space="preserve">Relation  E75.2 - 320  ist im BfArM nicht vorhanden </t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>P_1897170</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>E70.0</t>
+          <t>P_19285757</t>
         </is>
       </c>
       <c r="C7">
-        <v>79254</v>
+        <v>586</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Relation  E70.0 - 79254  ist im BfArM nicht vorhanden </t>
+          <t xml:space="preserve">Fehlendes ICD10 Code  </t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>P_19285751</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>E84.0</t>
+          <t>P_19285758</t>
         </is>
       </c>
       <c r="C8">
@@ -516,171 +506,58 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Relation  E84.0 - 587  ist im BfArM nicht vorhanden </t>
+          <t xml:space="preserve">Orpha Kodierung  587  ist im BfArM-Mapping nicht enthalten Fehlendes ICD10 Code  </t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>P_19285752</t>
+          <t>P_19285759</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>E84.8</t>
-        </is>
-      </c>
-      <c r="C9">
-        <v>586</v>
+          <t>E75.2</t>
+        </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Relation  E84.8 - 586  ist im BfArM nicht vorhanden</t>
+          <t xml:space="preserve">ICD10-Kodierung nicht eindeutig E75.2 Fehlendes Orpha_Kode  </t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>P_19285753</t>
+          <t>P_19285759</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>E84.8</t>
-        </is>
-      </c>
-      <c r="C10">
-        <v>587</v>
+          <t>E84.0</t>
+        </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t xml:space="preserve">ICD10 Kodierung  E84.8  ist im BfArm-Mapping nicht enthalten </t>
+          <t xml:space="preserve">Fehlendes Orpha_Kode  </t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>P_19285754</t>
+          <t>P_19285759</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>E85.0</t>
-        </is>
-      </c>
-      <c r="C11">
-        <v>586</v>
+          <t>D45</t>
+        </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Relation  E85.0 - 586  ist im BfArM nicht vorhanden </t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>P_19285755</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>E75.2</t>
-        </is>
-      </c>
-      <c r="C12">
-        <v>325</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Relation  E75.2 - 325  ist im BfArM nicht vorhanden </t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>P_19285756</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>E75.2</t>
-        </is>
-      </c>
-      <c r="C13">
-        <v>320</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Relation  E75.2 - 320  ist im BfArM nicht vorhanden </t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>P_19285757</t>
-        </is>
-      </c>
-      <c r="C14">
-        <v>586</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Fehlendes ICD10 Code  </t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>P_19285758</t>
-        </is>
-      </c>
-      <c r="C15">
-        <v>587</v>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Orpha Kodierung  587  ist im BfArM-Mapping nicht enthalten Fehlendes ICD10 Code  </t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>P_19285759</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>E75.2</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ICD10-Kodierung nicht eindeutig E75.2 </t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>P_19285759</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>E84.0</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ICD10-Kodierung nicht eindeutig E84.0 </t>
+          <t xml:space="preserve">Fehlendes Orpha_Kode  </t>
         </is>
       </c>
     </row>
@@ -741,19 +618,19 @@
         </is>
       </c>
       <c r="B2">
-        <v>0.11</v>
+        <v>0.28</v>
       </c>
       <c r="C2">
-        <v>99.89</v>
+        <v>99.72</v>
       </c>
       <c r="D2">
-        <v>94.44</v>
+        <v>90.62</v>
       </c>
       <c r="E2">
-        <v>96.59999999999999</v>
+        <v>98.3</v>
       </c>
       <c r="F2">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G2">
         <v>382</v>

</xml_diff>

<commit_message>
add extended number of RDs
</commit_message>
<xml_diff>
--- a/examples/Data/Export/Datenqualitätsreport_ CORD_TestData .xlsx
+++ b/examples/Data/Export/Datenqualitätsreport_ CORD_TestData .xlsx
@@ -568,7 +568,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -607,6 +607,11 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>icdRd_no_ext</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>pt_no</t>
         </is>
       </c>
@@ -633,6 +638,9 @@
         <v>32</v>
       </c>
       <c r="G2">
+        <v>297</v>
+      </c>
+      <c r="H2">
         <v>382</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add RD case number
</commit_message>
<xml_diff>
--- a/examples/Data/Export/Datenqualitätsreport_ CORD_TestData .xlsx
+++ b/examples/Data/Export/Datenqualitätsreport_ CORD_TestData .xlsx
@@ -391,10 +391,8 @@
           <t>E84.0</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>587</t>
-        </is>
+      <c r="C2">
+        <v>587</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -413,10 +411,8 @@
           <t>E84.80</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>587</t>
-        </is>
+      <c r="C3">
+        <v>587</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -435,10 +431,8 @@
           <t>E85.0</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>586</t>
-        </is>
+      <c r="C4">
+        <v>586</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -457,10 +451,8 @@
           <t>E75.2</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>325</t>
-        </is>
+      <c r="C5">
+        <v>325</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -479,10 +471,8 @@
           <t>E75.2</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>320</t>
-        </is>
+      <c r="C6">
+        <v>320</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -496,10 +486,8 @@
           <t>P_19285757</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>586</t>
-        </is>
+      <c r="C7">
+        <v>586</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -513,10 +501,8 @@
           <t>P_19285758</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>587</t>
-        </is>
+      <c r="C8">
+        <v>587</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -535,11 +521,6 @@
           <t>E75.2</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
       <c r="D9" t="inlineStr">
         <is>
           <t xml:space="preserve">ICD10-Kodierung nicht eindeutig E75.2 Fehlendes Orpha_Kode  </t>
@@ -557,11 +538,6 @@
           <t>E84.0</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
       <c r="D10" t="inlineStr">
         <is>
           <t xml:space="preserve">Fehlendes Orpha_Kode  </t>
@@ -579,11 +555,6 @@
           <t>D45</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
       <c r="D11" t="inlineStr">
         <is>
           <t xml:space="preserve">Fehlendes Orpha_Kode  </t>
@@ -601,11 +572,6 @@
           <t>J09</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
       <c r="D12" t="inlineStr">
         <is>
           <t xml:space="preserve">ICD10-Kodierung nicht eindeutig J09 </t>
@@ -616,11 +582,6 @@
       <c r="A13" t="inlineStr">
         <is>
           <t>P_19285759</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -636,7 +597,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -683,6 +644,11 @@
           <t>pt_no</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>case_no</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -700,16 +666,19 @@
         <v>90.62</v>
       </c>
       <c r="E2">
-        <v>98.3</v>
+        <v>97.7</v>
       </c>
       <c r="F2">
         <v>32</v>
       </c>
       <c r="G2">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="H2">
         <v>382</v>
+      </c>
+      <c r="I2">
+        <v>394</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated code and test data
</commit_message>
<xml_diff>
--- a/examples/Data/Export/Datenqualitätsreport_ CORD_TestData .xlsx
+++ b/examples/Data/Export/Datenqualitätsreport_ CORD_TestData .xlsx
@@ -352,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -383,67 +383,67 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>P_19285751</t>
+          <t>P_20085751</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>E84.0</t>
+          <t>G70</t>
         </is>
       </c>
       <c r="C2">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Relation  E84.0 - 587  ist im BfArM nicht vorhanden </t>
+          <t>Relation  G70 - 586  ist im BfArM nicht vorhanden</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>P_19285753</t>
+          <t>P_20085752</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>E84.80</t>
+          <t>G70</t>
         </is>
       </c>
       <c r="C3">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Relation  E84.80 - 587  ist im BfArM nicht vorhanden </t>
+          <t>Relation  G70 - 589  ist im BfArM nicht vorhanden</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>P_19285754</t>
+          <t>P_20085754</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>E85.0</t>
+          <t>E84.80</t>
         </is>
       </c>
       <c r="C4">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Relation  E85.0 - 586  ist im BfArM nicht vorhanden </t>
+          <t xml:space="preserve">Relation  E84.80 - 588  ist im BfArM nicht vorhanden </t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>P_19285755</t>
+          <t>P_20085755</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -463,7 +463,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>P_19285756</t>
+          <t>P_20085756</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -483,7 +483,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>P_19285757</t>
+          <t>P_20085757</t>
         </is>
       </c>
       <c r="C7">
@@ -498,7 +498,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>P_19285758</t>
+          <t>P_20085758</t>
         </is>
       </c>
       <c r="C8">
@@ -513,29 +513,29 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>P_19285759</t>
+          <t>P_20085759</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>E75.2</t>
+          <t>E84.0</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t xml:space="preserve">ICD10-Kodierung nicht eindeutig E75.2 Fehlendes Orpha_Kode  </t>
+          <t xml:space="preserve">Fehlendes Orpha_Kode  </t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>P_19285759</t>
+          <t>P_20085760</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>E84.0</t>
+          <t>D45</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -547,46 +547,103 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>P_19285759</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>D45</t>
+          <t>P_20085761</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fehlendes Orpha_Kode  </t>
+          <t xml:space="preserve">Fehlendes ICD10 Code  </t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>P_19285759</t>
+          <t>P_20085762</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>J09</t>
-        </is>
+          <t>E66.89</t>
+        </is>
+      </c>
+      <c r="C12">
+        <v>320</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t xml:space="preserve">ICD10-Kodierung nicht eindeutig J09 </t>
+          <t xml:space="preserve">Relation  E66.89 - 320  ist im BfArM nicht vorhanden </t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>P_19285759</t>
+          <t>P_20085764</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>E66.89</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fehlendes ICD10 Code  </t>
+          <t xml:space="preserve">ICD10-Kodierung nicht eindeutig E66.89 Fehlendes Orpha_Kode  </t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>P_20085764</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>E75.2</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ICD10-Kodierung nicht eindeutig E75.2 Fehlendes Orpha_Kode  </t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>P_20085767</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>E85.0</t>
+        </is>
+      </c>
+      <c r="C15">
+        <v>586</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Relation  E85.0 - 586  ist im BfArM nicht vorhanden </t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>P_20085770</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>J09</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ICD10-Kodierung nicht eindeutig J09 </t>
         </is>
       </c>
     </row>
@@ -657,28 +714,28 @@
         </is>
       </c>
       <c r="B2">
-        <v>0.34</v>
+        <v>15.47</v>
       </c>
       <c r="C2">
-        <v>99.66</v>
+        <v>84.53</v>
       </c>
       <c r="D2">
-        <v>90.62</v>
+        <v>88.23999999999999</v>
       </c>
       <c r="E2">
-        <v>97.7</v>
+        <v>97.40000000000001</v>
       </c>
       <c r="F2">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G2">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="H2">
-        <v>382</v>
+        <v>395</v>
       </c>
       <c r="I2">
-        <v>394</v>
+        <v>420</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update dq_msg and umlauts
</commit_message>
<xml_diff>
--- a/examples/Data/Export/Datenqualitätsreport_ CORD_TestData .xlsx
+++ b/examples/Data/Export/Datenqualitätsreport_ CORD_TestData .xlsx
@@ -352,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -366,7 +366,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>ICD_Primärkode</t>
+          <t>ICD_primaerkode</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -396,7 +396,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Relation  G70 - 586  ist im BfArM nicht vorhanden</t>
+          <t xml:space="preserve">Kodierung nicht eindeutig. Relation G70 - 586 ist im BfArM nicht vorhanden. </t>
         </is>
       </c>
     </row>
@@ -416,7 +416,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Relation  G70 - 589  ist im BfArM nicht vorhanden</t>
+          <t xml:space="preserve">Kodierung nicht eindeutig. Relation G70 - 589 ist im BfArM nicht vorhanden. </t>
         </is>
       </c>
     </row>
@@ -436,7 +436,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Relation  E84.80 - 588  ist im BfArM nicht vorhanden </t>
+          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E84.80 - 588 ist im BfArM nicht vorhanden.  </t>
         </is>
       </c>
     </row>
@@ -456,7 +456,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Relation  E75.2 - 325  ist im BfArM nicht vorhanden </t>
+          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E75.2 - 325 ist im BfArM nicht vorhanden.  </t>
         </is>
       </c>
     </row>
@@ -476,7 +476,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Relation  E75.2 - 320  ist im BfArM nicht vorhanden </t>
+          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E75.2 - 320 ist im BfArM nicht vorhanden.  </t>
         </is>
       </c>
     </row>
@@ -491,7 +491,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fehlendes ICD10 Code  </t>
+          <t xml:space="preserve">Fehlendes ICD10 Code.  </t>
         </is>
       </c>
     </row>
@@ -506,7 +506,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Orpha Kodierung  587  ist im BfArM-Mapping nicht enthalten Fehlendes ICD10 Code  </t>
+          <t xml:space="preserve">Orpha Kodierung 587 ist im BfArM-Mapping nicht enthalten.  Fehlendes ICD10 Code.  </t>
         </is>
       </c>
     </row>
@@ -523,7 +523,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fehlendes Orpha_Kode  </t>
+          <t xml:space="preserve">Fehlendes Orpha_Kode.  </t>
         </is>
       </c>
     </row>
@@ -540,7 +540,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fehlendes Orpha_Kode  </t>
+          <t xml:space="preserve">Fehlendes Orpha_Kode.  </t>
         </is>
       </c>
     </row>
@@ -552,7 +552,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fehlendes ICD10 Code  </t>
+          <t xml:space="preserve">Fehlendes ICD10 Code.  </t>
         </is>
       </c>
     </row>
@@ -572,7 +572,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Relation  E66.89 - 320  ist im BfArM nicht vorhanden </t>
+          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E66.89 - 320 ist im BfArM nicht vorhanden.  </t>
         </is>
       </c>
     </row>
@@ -589,7 +589,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t xml:space="preserve">ICD10-Kodierung nicht eindeutig E66.89 Fehlendes Orpha_Kode  </t>
+          <t xml:space="preserve">Fehlendes Orpha_Kode.  </t>
         </is>
       </c>
     </row>
@@ -606,7 +606,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t xml:space="preserve">ICD10-Kodierung nicht eindeutig E75.2 Fehlendes Orpha_Kode  </t>
+          <t xml:space="preserve">Fehlendes Orpha_Kode.  </t>
         </is>
       </c>
     </row>
@@ -626,24 +626,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Relation  E85.0 - 586  ist im BfArM nicht vorhanden </t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>P_20085770</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>J09</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ICD10-Kodierung nicht eindeutig J09 </t>
+          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E85.0 - 586 ist im BfArM nicht vorhanden.  </t>
         </is>
       </c>
     </row>
@@ -688,12 +671,12 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>icdRd_no</t>
+          <t>K2_icdRd_no</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>icdRd_no_ext</t>
+          <t>K3_rd_no</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -723,13 +706,13 @@
         <v>88.23999999999999</v>
       </c>
       <c r="E2">
-        <v>97.40000000000001</v>
+        <v>97.7</v>
       </c>
       <c r="F2">
         <v>34</v>
       </c>
       <c r="G2">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="H2">
         <v>395</v>

</xml_diff>

<commit_message>
update checkCordDQ and reports
</commit_message>
<xml_diff>
--- a/examples/Data/Export/Datenqualitätsreport_ CORD_TestData .xlsx
+++ b/examples/Data/Export/Datenqualitätsreport_ CORD_TestData .xlsx
@@ -396,7 +396,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Kodierung nicht eindeutig. Relation G70 - 586 ist im BfArM nicht vorhanden. </t>
+          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation G70 - 586 ist im BfArM nicht vorhanden. </t>
         </is>
       </c>
     </row>
@@ -416,7 +416,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Kodierung nicht eindeutig. Relation G70 - 589 ist im BfArM nicht vorhanden. </t>
+          <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation G70 - 589 ist im BfArM nicht vorhanden. </t>
         </is>
       </c>
     </row>
@@ -589,7 +589,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fehlendes Orpha_Kode.  </t>
+          <t xml:space="preserve">ICD10 Kodierung E66.89 ist nicht eindeutig. ICD10-Orpha Relation ist gemäß Tracer-Diagnosenliste vom Typ 1-m.  Fehlendes Orpha_Kode.  </t>
         </is>
       </c>
     </row>
@@ -606,7 +606,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fehlendes Orpha_Kode.  </t>
+          <t xml:space="preserve">ICD10 Kodierung E75.2 ist nicht eindeutig. ICD10-Orpha Relation ist gemäß Tracer-Diagnosenliste vom Typ 1-m.  Fehlendes Orpha_Kode.  </t>
         </is>
       </c>
     </row>
@@ -706,7 +706,7 @@
         <v>88.23999999999999</v>
       </c>
       <c r="E2">
-        <v>97.7</v>
+        <v>97.09999999999999</v>
       </c>
       <c r="F2">
         <v>34</v>

</xml_diff>

<commit_message>
added institut ID and case ID to DQ Reports
</commit_message>
<xml_diff>
--- a/examples/Data/Export/Datenqualitätsreport_ CORD_TestData .xlsx
+++ b/examples/Data/Export/Datenqualitätsreport_ CORD_TestData .xlsx
@@ -352,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -366,15 +366,20 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Aufnahmenummer</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>ICD_primaerkode</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Orpha_Kode</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>dq_msg</t>
         </is>
@@ -388,13 +393,18 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>F_101645</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>G70</t>
         </is>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>586</v>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation G70 - 586 ist im BfArM nicht vorhanden. </t>
         </is>
@@ -408,13 +418,18 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>F_101646</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>G70</t>
         </is>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>589</v>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation G70 - 589 ist im BfArM nicht vorhanden. </t>
         </is>
@@ -428,13 +443,18 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>F_101648</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>E84.80</t>
         </is>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>588</v>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E84.80 - 588 ist im BfArM nicht vorhanden.  </t>
         </is>
@@ -448,13 +468,18 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>F_101649</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>E75.2</t>
         </is>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>325</v>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E75.2 - 325 ist im BfArM nicht vorhanden.  </t>
         </is>
@@ -468,13 +493,18 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>F_101650</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>E75.2</t>
         </is>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>320</v>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E75.2 - 320 ist im BfArM nicht vorhanden.  </t>
         </is>
@@ -486,10 +516,15 @@
           <t>P_20085757</t>
         </is>
       </c>
-      <c r="C7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>F_101651</t>
+        </is>
+      </c>
+      <c r="D7">
         <v>586</v>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t xml:space="preserve">Fehlendes ICD10 Code.  </t>
         </is>
@@ -501,10 +536,15 @@
           <t>P_20085758</t>
         </is>
       </c>
-      <c r="C8">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>F_101651</t>
+        </is>
+      </c>
+      <c r="D8">
         <v>587</v>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t xml:space="preserve">Orpha Kodierung 587 ist im BfArM-Mapping nicht enthalten.  Fehlendes ICD10 Code.  </t>
         </is>
@@ -518,10 +558,15 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>F_101653</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>E84.0</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t xml:space="preserve">Fehlendes Orpha_Kode.  </t>
         </is>
@@ -535,10 +580,15 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>F_101654</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
           <t>D45</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t xml:space="preserve">Fehlendes Orpha_Kode.  </t>
         </is>
@@ -550,7 +600,12 @@
           <t>P_20085761</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>F_101655</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
         <is>
           <t xml:space="preserve">Fehlendes ICD10 Code.  </t>
         </is>
@@ -564,13 +619,18 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>F_101656</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
           <t>E66.89</t>
         </is>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>320</v>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E66.89 - 320 ist im BfArM nicht vorhanden.  </t>
         </is>
@@ -584,10 +644,15 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>F_101757</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
           <t>E66.89</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t xml:space="preserve">ICD10 Kodierung E66.89 ist nicht eindeutig. ICD10-Orpha Relation ist gemäß Tracer-Diagnosenliste vom Typ 1-m.  Fehlendes Orpha_Kode.  </t>
         </is>
@@ -601,10 +666,15 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>F_101658</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
           <t>E75.2</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t xml:space="preserve">ICD10 Kodierung E75.2 ist nicht eindeutig. ICD10-Orpha Relation ist gemäß Tracer-Diagnosenliste vom Typ 1-m.  Fehlendes Orpha_Kode.  </t>
         </is>
@@ -618,13 +688,18 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>F_101660</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
           <t>E85.0</t>
         </is>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>586</v>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t xml:space="preserve">Kodierung ist nicht eindeutig. Relation E85.0 - 586 ist im BfArM nicht vorhanden.  </t>
         </is>
@@ -646,7 +721,7 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>basicItem</t>
+          <t>inst_id</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -693,14 +768,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Total</t>
+          <t>260123430-Dali</t>
         </is>
       </c>
       <c r="B2">
-        <v>15.47</v>
+        <v>3.13</v>
       </c>
       <c r="C2">
-        <v>84.53</v>
+        <v>96.87</v>
       </c>
       <c r="D2">
         <v>88.23999999999999</v>

</xml_diff>